<commit_message>
added some room descriptions
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EwanS\Documents\Revature\HomeTour\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA94F4D7-3AF5-42C7-B8D1-20B59C7E6950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE8A15B-5554-4877-BB55-A0D9CFD25821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{047D2535-50AE-4626-A6D8-1AC5B1CF15CA}"/>
   </bookViews>
@@ -34,16 +34,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>starting</t>
+    <t>end</t>
+  </si>
+  <si>
+    <t>start</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,8 +61,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -71,8 +82,13 @@
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -95,16 +111,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -418,27 +452,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D708928-11EF-406B-A5BD-8D38600BCF9E}">
-  <dimension ref="A2:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
+    <row r="5" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added descriptions, key implementation
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EwanS\Documents\Revature\HomeTour\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE8A15B-5554-4877-BB55-A0D9CFD25821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A88548C-FC1C-4D68-BAD1-F9A972FD4454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{047D2535-50AE-4626-A6D8-1AC5B1CF15CA}"/>
   </bookViews>
@@ -455,7 +455,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,14 +475,14 @@
     <row r="3" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>